<commit_message>
Fini question 2-3, ajout nelson
</commit_message>
<xml_diff>
--- a/eurf.xlsx
+++ b/eurf.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbela\Downloads\Data_Excel\Data_Excel\MSCI_ESGscores\FF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbela\ecole\FIN-429-Sustainable-finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133A9703-BA79-4650-9FF6-1C28809FCFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACD0D48-08CA-4C73-BE0D-770C3708BC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1428" yWindow="1476" windowWidth="17280" windowHeight="9960" xr2:uid="{50FC72A7-C13A-4AA5-ADA7-E409A5B38808}"/>
   </bookViews>

</xml_diff>